<commit_message>
checks percentage of matches with manual sample
</commit_message>
<xml_diff>
--- a/Registration Numbers.xlsx
+++ b/Registration Numbers.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -444,7 +444,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>20th Century Boy</t>
+          <t>13463-20th Century Boy</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -459,7 +459,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>WHO ARE YOU</t>
+          <t>54307-WHO ARE YOU</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -474,7 +474,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BABA O'RILEY</t>
+          <t>56418-BABA O'RILEY</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -489,7 +489,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>MEANT TO BE</t>
+          <t>191848-MEANT TO BE</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -500,614 +500,524 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t xml:space="preserve">HUMBLE AND KIND </t>
+          <t>191897-SOUTHBOUND</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>PA0002127076</t>
+          <t>PA0002267459</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>SOUTHBOUND</t>
+          <t>202993-BEER NEVER BROKE MY HEART</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>PA0002267459</t>
+          <t>PA0002192567</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BEER NEVER BROKE MY HEART</t>
+          <t>24776-CAN'T YOU SEE U.S. ONLY AS OF)</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>PA0002192567</t>
+          <t>SR0000863063</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t xml:space="preserve">HOLIDAY </t>
+          <t>19819-20th Century Boy - Master</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>PA0001041153</t>
+          <t>SR0000233398</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t xml:space="preserve">20th Century Boy </t>
+          <t>11872-Heaven Is A Place On Earth</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>PA0000877899</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Heaven Is A Place On Earth</t>
+          <t>56421-BEHIND BLUE EYES</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>PA0000877899</t>
+          <t>PA0000347339</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BEHIND BLUE EYES</t>
+          <t>56531-PINBALL WIZARD</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>PA0000347339</t>
+          <t>PA0000750495</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>PINBALL WIZARD</t>
+          <t>13262-Children Of The Revolution</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>PA0000750495</t>
+          <t>PA0001015278</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Children Of The Revolution</t>
+          <t>191840-LOVE WINS</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>PA0001015278</t>
+          <t>PA0002031121</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t xml:space="preserve">HIGHWAY DON'T CARE </t>
+          <t>1943-GONNA MAKE YOU SWEAT</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>PA0000520237</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>LOVE WINS</t>
+          <t>100056-TEACH YOUR CHILDREN</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>PA0002031121</t>
+          <t>V3615D973</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>GONNA MAKE YOU SWEAT</t>
+          <t>12008-You Get What You Give</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>PA0000520237</t>
+          <t>V3615D973</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>TEACH YOUR CHILDREN</t>
+          <t>191644-DRINKING ALONE</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>V3615D973</t>
+          <t>PA0002233922</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>You Get What You Give</t>
+          <t>182638-BODY LIKE A BACK ROAD</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>V3615D973</t>
+          <t>PA0002067268</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>DRINKING ALONE</t>
+          <t>56635-MY GENERATION</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>PA0002233922</t>
+          <t>PA0000722088</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BODY LIKE A BACK ROAD</t>
+          <t>165764-THIS IS IT</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>PA0002067268</t>
+          <t>PA0001618358</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t xml:space="preserve">25 OR 6 TO 4 </t>
+          <t>56469-THE SEEKER</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>PA0001719331</t>
+          <t>PA0002029207</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>MY GENERATION</t>
+          <t>190499-THE WAY I AM</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>PA0000722088</t>
+          <t>PA0001601324</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>THIS IS IT</t>
+          <t>56584-JOIN TOGETHER</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>PA0001618358</t>
+          <t>PA0001218253</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t xml:space="preserve">DANCE HALL DAYS </t>
+          <t>149616-CHA CHA SLIDE</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>PA0000215280</t>
+          <t>PA0001204600</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>THE SEEKER</t>
+          <t>12188-DANCE HALL DAYS</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>PA0002029207</t>
+          <t>PA0001074195</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>THE WAY I AM</t>
+          <t>NL50499-TOMMY - STAGE INCOME</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>PA0001601324</t>
+          <t>PA0000539941</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>27</v>
+        <v>38</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>JOIN TOGETHER</t>
+          <t>56638-I'M A BOY</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>PA0001218253</t>
+          <t>PA0001218257</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CHA CHA SLIDE</t>
+          <t>12203-EVERYBODY HAVE FUN TONIGHT</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>PA0001204600</t>
+          <t>PA0000324723</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t xml:space="preserve">SHOTGUN RIDER </t>
+          <t>480-CHRISTMAS WRAPPING</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>PA0001938938</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>DANCE HALL DAYS</t>
+          <t>193999-HERE AND NOW</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>PA0001074195</t>
+          <t>PA0000394195</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BODY</t>
+          <t>10841-FAMILY AFFAIR BOTH SHARES)</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>PA0001800681</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t xml:space="preserve">TOMMY </t>
+          <t>92403-BAREFOOT BLUE JEAN NIGHT BMI</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>PA0000539941</t>
+          <t>SR0000697851</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>I'M A BOY</t>
+          <t>182982-SUNRISE SUNBURN SUNSET</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>PA0001218257</t>
+          <t>PA0002140607</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>EVERYBODY HAVE FUN TONIGHT</t>
+          <t>187657-GOOD VIBES</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PA0000324723</t>
+          <t>PA0002228161</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>CHRISTMAS WRAPPING</t>
+          <t>187820-RIDIN' ROADS</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>PA0002197474</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>HERE AND NOW</t>
+          <t>203068-I HOPE YOU'RE HAPPY NOW</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>PA0000394195</t>
+          <t>PA0002297072</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>37</v>
+        <v>48</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t xml:space="preserve">FAMILY AFFAIR </t>
+          <t>1522-LET'S TWIST AGAIN</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>SRu001415475</t>
+          <t>PA0000196738</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>38</v>
+        <v>49</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t xml:space="preserve">BAREFOOT BLUE JEAN NIGHT </t>
+          <t>20839-I Know You Want Me</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>PA0001793292</t>
+          <t>TX0002685123</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>39</v>
+        <v>50</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>SUNRISE SUNBURN SUNSET</t>
+          <t>54313-EMINENCE FRONT</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="n">
-        <v>40</v>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>GOOD VIBES</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>PA0002228161</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="n">
-        <v>41</v>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>RIDIN' ROADS</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>PA0002197474</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="n">
-        <v>42</v>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>I HOPE YOU'RE HAPPY NOW</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>PA0002297072</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="n">
-        <v>43</v>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>LET'S TWIST AGAIN</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>PA0000196738</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="n">
-        <v>44</v>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>I Know You Want Me</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>TX0002685123</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="n">
-        <v>45</v>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>EMINENCE FRONT</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
         <is>
           <t>PA0000152030</t>
         </is>

</xml_diff>